<commit_message>
Another try on vectors
</commit_message>
<xml_diff>
--- a/data/input_data/UpdatedMeanVectors.xlsx
+++ b/data/input_data/UpdatedMeanVectors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erichare/GitHub/major-me/data/input_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE293723-1206-6744-BE7A-777D48413A61}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C6E5A16-2674-5B44-9006-59B082775658}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5380" yWindow="2200" windowWidth="33780" windowHeight="19020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5380" yWindow="2200" windowWidth="33780" windowHeight="19020" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="47">
   <si>
     <t>Numeracy</t>
   </si>
@@ -169,6 +169,9 @@
   </si>
   <si>
     <t>Open to Experience</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -2502,8 +2505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2617,7 +2620,7 @@
       </c>
       <c r="F3" s="1">
         <f>VLOOKUP(A3,'Lawrence Lookups'!M:N,2,FALSE)</f>
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="G3" s="1">
         <f>VLOOKUP('Lawernce Mean Vectors'!A3,'Lawrence Lookups'!P:Q,2,FALSE)</f>
@@ -2658,7 +2661,7 @@
       </c>
       <c r="F4" s="1">
         <f>VLOOKUP(A4,'Lawrence Lookups'!M:N,2,FALSE)</f>
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="G4" s="1">
         <f>VLOOKUP('Lawernce Mean Vectors'!A4,'Lawrence Lookups'!P:Q,2,FALSE)</f>
@@ -2740,7 +2743,7 @@
       </c>
       <c r="F6" s="1">
         <f>VLOOKUP(A6,'Lawrence Lookups'!M:N,2,FALSE)</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G6" s="1">
         <f>VLOOKUP('Lawernce Mean Vectors'!A6,'Lawrence Lookups'!P:Q,2,FALSE)</f>
@@ -2822,7 +2825,7 @@
       </c>
       <c r="F8" s="1">
         <f>VLOOKUP(A8,'Lawrence Lookups'!M:N,2,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" s="1">
         <f>VLOOKUP('Lawernce Mean Vectors'!A8,'Lawrence Lookups'!P:Q,2,FALSE)</f>
@@ -2863,7 +2866,7 @@
       </c>
       <c r="F9" s="1">
         <f>VLOOKUP(A9,'Lawrence Lookups'!M:N,2,FALSE)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="G9" s="1">
         <f>VLOOKUP('Lawernce Mean Vectors'!A9,'Lawrence Lookups'!P:Q,2,FALSE)</f>
@@ -2904,7 +2907,7 @@
       </c>
       <c r="F10" s="1">
         <f>VLOOKUP(A10,'Lawrence Lookups'!M:N,2,FALSE)</f>
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="G10" s="1">
         <f>VLOOKUP('Lawernce Mean Vectors'!A10,'Lawrence Lookups'!P:Q,2,FALSE)</f>
@@ -2945,7 +2948,7 @@
       </c>
       <c r="F11" s="1">
         <f>VLOOKUP(A11,'Lawrence Lookups'!M:N,2,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11" s="1">
         <f>VLOOKUP('Lawernce Mean Vectors'!A11,'Lawrence Lookups'!P:Q,2,FALSE)</f>
@@ -3191,7 +3194,7 @@
       </c>
       <c r="F17" s="1">
         <f>VLOOKUP(A17,'Lawrence Lookups'!M:N,2,FALSE)</f>
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="G17" s="1">
         <f>VLOOKUP('Lawernce Mean Vectors'!A17,'Lawrence Lookups'!P:Q,2,FALSE)</f>
@@ -3569,10 +3572,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:Z25"/>
+  <dimension ref="A1:Z43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S32" sqref="S32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4284,7 +4287,7 @@
         <v>1</v>
       </c>
       <c r="M13" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="N13">
         <v>1</v>
@@ -4340,7 +4343,7 @@
         <v>1</v>
       </c>
       <c r="M14" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="N14">
         <v>1</v>
@@ -4396,10 +4399,10 @@
         <v>1</v>
       </c>
       <c r="M15" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="N15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P15" t="s">
         <v>20</v>
@@ -4452,7 +4455,7 @@
         <v>0</v>
       </c>
       <c r="M16" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="N16">
         <v>0</v>
@@ -4508,7 +4511,7 @@
         <v>0</v>
       </c>
       <c r="M17" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="N17">
         <v>0</v>
@@ -4564,7 +4567,7 @@
         <v>0</v>
       </c>
       <c r="M18" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="N18">
         <v>0</v>
@@ -4620,7 +4623,7 @@
         <v>0</v>
       </c>
       <c r="M19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N19">
         <v>0</v>
@@ -4676,10 +4679,10 @@
         <v>0</v>
       </c>
       <c r="M20" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="N20">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="P20" t="s">
         <v>11</v>
@@ -4732,10 +4735,10 @@
         <v>-1</v>
       </c>
       <c r="M21" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="N21">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="P21" t="s">
         <v>12</v>
@@ -4788,7 +4791,7 @@
         <v>-1</v>
       </c>
       <c r="M22" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N22">
         <v>-1</v>
@@ -4844,7 +4847,7 @@
         <v>-1</v>
       </c>
       <c r="M23" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="N23">
         <v>-1</v>
@@ -4900,7 +4903,7 @@
         <v>-2</v>
       </c>
       <c r="M24" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="N24">
         <v>-2</v>
@@ -4956,7 +4959,7 @@
         <v>-2</v>
       </c>
       <c r="M25" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="N25">
         <v>-2</v>
@@ -4984,6 +4987,11 @@
       </c>
       <c r="Z25">
         <v>-2</v>
+      </c>
+    </row>
+    <row r="43" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J43" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
merged social studies with sociology rounded 1.5 to 2
</commit_message>
<xml_diff>
--- a/data/input_data/UpdatedMeanVectors.xlsx
+++ b/data/input_data/UpdatedMeanVectors.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erichare/GitHub/major-me/data/input_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nadia/Documents/GitHub/smart-match/data/input_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C6E5A16-2674-5B44-9006-59B082775658}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DFE43E4-2319-0645-8B22-F18ECCA744C8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5380" yWindow="2200" windowWidth="33780" windowHeight="19020" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15740" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="48">
   <si>
     <t>Numeracy</t>
   </si>
@@ -172,6 +172,9 @@
   </si>
   <si>
     <t>s</t>
+  </si>
+  <si>
+    <t>Social Science</t>
   </si>
 </sst>
 </file>
@@ -588,7 +591,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:J32"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2503,10 +2506,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2780,7 +2783,7 @@
       </c>
       <c r="E7" s="1">
         <f>VLOOKUP(A7,'Lawrence Lookups'!J:K,2,FALSE)</f>
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="F7" s="1">
         <f>VLOOKUP(A7,'Lawrence Lookups'!M:N,2,FALSE)</f>
@@ -2846,7 +2849,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="B9" s="1">
         <f>VLOOKUP(A9,'Lawrence Lookups'!A:B,2,FALSE)</f>
@@ -3051,7 +3054,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B14" s="1">
         <f>VLOOKUP(A14,'Lawrence Lookups'!A:B,2,FALSE)</f>
@@ -3063,7 +3066,7 @@
       </c>
       <c r="D14" s="1">
         <f>VLOOKUP(A14,'Lawrence Lookups'!G:H,2,FALSE)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E14" s="1">
         <f>VLOOKUP(A14,'Lawrence Lookups'!J:K,2,FALSE)</f>
@@ -3079,7 +3082,7 @@
       </c>
       <c r="H14" s="1">
         <f>VLOOKUP(A14,'Lawrence Lookups'!S:T,2,FALSE)</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I14" s="1">
         <f>VLOOKUP(A14,'Lawrence Lookups'!V:W,2,FALSE)</f>
@@ -3092,31 +3095,31 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B15" s="1">
         <f>VLOOKUP(A15,'Lawrence Lookups'!A:B,2,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" s="1">
         <f>VLOOKUP(A15,'Lawrence Lookups'!D:E,2,FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15" s="1">
         <f>VLOOKUP(A15,'Lawrence Lookups'!G:H,2,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" s="1">
         <f>VLOOKUP(A15,'Lawrence Lookups'!J:K,2,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F15" s="1">
         <f>VLOOKUP(A15,'Lawrence Lookups'!M:N,2,FALSE)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G15" s="1">
         <f>VLOOKUP('Lawernce Mean Vectors'!A15,'Lawrence Lookups'!P:Q,2,FALSE)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H15" s="1">
         <f>VLOOKUP(A15,'Lawrence Lookups'!S:T,2,FALSE)</f>
@@ -3128,12 +3131,12 @@
       </c>
       <c r="J15" s="1">
         <f>VLOOKUP(A15,'Lawrence Lookups'!Y:Z,2,FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B16" s="1">
         <f>VLOOKUP(A16,'Lawrence Lookups'!A:B,2,FALSE)</f>
@@ -3145,7 +3148,7 @@
       </c>
       <c r="D16" s="1">
         <f>VLOOKUP(A16,'Lawrence Lookups'!G:H,2,FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16" s="1">
         <f>VLOOKUP(A16,'Lawrence Lookups'!J:K,2,FALSE)</f>
@@ -3153,7 +3156,7 @@
       </c>
       <c r="F16" s="1">
         <f>VLOOKUP(A16,'Lawrence Lookups'!M:N,2,FALSE)</f>
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="G16" s="1">
         <f>VLOOKUP('Lawernce Mean Vectors'!A16,'Lawrence Lookups'!P:Q,2,FALSE)</f>
@@ -3161,7 +3164,7 @@
       </c>
       <c r="H16" s="1">
         <f>VLOOKUP(A16,'Lawrence Lookups'!S:T,2,FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I16" s="1">
         <f>VLOOKUP(A16,'Lawrence Lookups'!V:W,2,FALSE)</f>
@@ -3174,7 +3177,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B17" s="1">
         <f>VLOOKUP(A17,'Lawrence Lookups'!A:B,2,FALSE)</f>
@@ -3186,7 +3189,7 @@
       </c>
       <c r="D17" s="1">
         <f>VLOOKUP(A17,'Lawrence Lookups'!G:H,2,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" s="1">
         <f>VLOOKUP(A17,'Lawrence Lookups'!J:K,2,FALSE)</f>
@@ -3194,7 +3197,7 @@
       </c>
       <c r="F17" s="1">
         <f>VLOOKUP(A17,'Lawrence Lookups'!M:N,2,FALSE)</f>
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="G17" s="1">
         <f>VLOOKUP('Lawernce Mean Vectors'!A17,'Lawrence Lookups'!P:Q,2,FALSE)</f>
@@ -3202,11 +3205,11 @@
       </c>
       <c r="H17" s="1">
         <f>VLOOKUP(A17,'Lawrence Lookups'!S:T,2,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17" s="1">
         <f>VLOOKUP(A17,'Lawrence Lookups'!V:W,2,FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17" s="1">
         <f>VLOOKUP(A17,'Lawrence Lookups'!Y:Z,2,FALSE)</f>
@@ -3215,23 +3218,23 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="B18" s="1">
         <f>VLOOKUP(A18,'Lawrence Lookups'!A:B,2,FALSE)</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C18" s="1">
         <f>VLOOKUP(A18,'Lawrence Lookups'!D:E,2,FALSE)</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D18" s="1">
         <f>VLOOKUP(A18,'Lawrence Lookups'!G:H,2,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E18" s="1">
         <f>VLOOKUP(A18,'Lawrence Lookups'!J:K,2,FALSE)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F18" s="1">
         <f>VLOOKUP(A18,'Lawrence Lookups'!M:N,2,FALSE)</f>
@@ -3239,24 +3242,24 @@
       </c>
       <c r="G18" s="1">
         <f>VLOOKUP('Lawernce Mean Vectors'!A18,'Lawrence Lookups'!P:Q,2,FALSE)</f>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="H18" s="1">
         <f>VLOOKUP(A18,'Lawrence Lookups'!S:T,2,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I18" s="1">
         <f>VLOOKUP(A18,'Lawrence Lookups'!V:W,2,FALSE)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J18" s="1">
         <f>VLOOKUP(A18,'Lawrence Lookups'!Y:Z,2,FALSE)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="B19" s="1">
         <f>VLOOKUP(A19,'Lawrence Lookups'!A:B,2,FALSE)</f>
@@ -3264,7 +3267,7 @@
       </c>
       <c r="C19" s="1">
         <f>VLOOKUP(A19,'Lawrence Lookups'!D:E,2,FALSE)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D19" s="1">
         <f>VLOOKUP(A19,'Lawrence Lookups'!G:H,2,FALSE)</f>
@@ -3280,15 +3283,15 @@
       </c>
       <c r="G19" s="1">
         <f>VLOOKUP('Lawernce Mean Vectors'!A19,'Lawrence Lookups'!P:Q,2,FALSE)</f>
-        <v>-2</v>
+        <v>1</v>
       </c>
       <c r="H19" s="1">
         <f>VLOOKUP(A19,'Lawrence Lookups'!S:T,2,FALSE)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I19" s="1">
         <f>VLOOKUP(A19,'Lawrence Lookups'!V:W,2,FALSE)</f>
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="J19" s="1">
         <f>VLOOKUP(A19,'Lawrence Lookups'!Y:Z,2,FALSE)</f>
@@ -3296,8 +3299,8 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>24</v>
+      <c r="A20" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B20" s="1">
         <f>VLOOKUP(A20,'Lawrence Lookups'!A:B,2,FALSE)</f>
@@ -3305,7 +3308,7 @@
       </c>
       <c r="C20" s="1">
         <f>VLOOKUP(A20,'Lawrence Lookups'!D:E,2,FALSE)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D20" s="1">
         <f>VLOOKUP(A20,'Lawrence Lookups'!G:H,2,FALSE)</f>
@@ -3317,19 +3320,19 @@
       </c>
       <c r="F20" s="1">
         <f>VLOOKUP(A20,'Lawrence Lookups'!M:N,2,FALSE)</f>
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="G20" s="1">
         <f>VLOOKUP('Lawernce Mean Vectors'!A20,'Lawrence Lookups'!P:Q,2,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H20" s="1">
         <f>VLOOKUP(A20,'Lawrence Lookups'!S:T,2,FALSE)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I20" s="1">
         <f>VLOOKUP(A20,'Lawrence Lookups'!V:W,2,FALSE)</f>
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="J20" s="1">
         <f>VLOOKUP(A20,'Lawrence Lookups'!Y:Z,2,FALSE)</f>
@@ -3337,16 +3340,16 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>41</v>
+      <c r="A21" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="B21" s="1">
         <f>VLOOKUP(A21,'Lawrence Lookups'!A:B,2,FALSE)</f>
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="C21" s="1">
         <f>VLOOKUP(A21,'Lawrence Lookups'!D:E,2,FALSE)</f>
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="D21" s="1">
         <f>VLOOKUP(A21,'Lawrence Lookups'!G:H,2,FALSE)</f>
@@ -3358,7 +3361,7 @@
       </c>
       <c r="F21" s="1">
         <f>VLOOKUP(A21,'Lawrence Lookups'!M:N,2,FALSE)</f>
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="G21" s="1">
         <f>VLOOKUP('Lawernce Mean Vectors'!A21,'Lawrence Lookups'!P:Q,2,FALSE)</f>
@@ -3374,12 +3377,12 @@
       </c>
       <c r="J21" s="1">
         <f>VLOOKUP(A21,'Lawrence Lookups'!Y:Z,2,FALSE)</f>
-        <v>-1</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B22" s="1">
         <f>VLOOKUP(A22,'Lawrence Lookups'!A:B,2,FALSE)</f>
@@ -3387,7 +3390,7 @@
       </c>
       <c r="C22" s="1">
         <f>VLOOKUP(A22,'Lawrence Lookups'!D:E,2,FALSE)</f>
-        <v>-2</v>
+        <v>1</v>
       </c>
       <c r="D22" s="1">
         <f>VLOOKUP(A22,'Lawrence Lookups'!G:H,2,FALSE)</f>
@@ -3403,7 +3406,7 @@
       </c>
       <c r="G22" s="1">
         <f>VLOOKUP('Lawernce Mean Vectors'!A22,'Lawrence Lookups'!P:Q,2,FALSE)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H22" s="1">
         <f>VLOOKUP(A22,'Lawrence Lookups'!S:T,2,FALSE)</f>
@@ -3411,7 +3414,7 @@
       </c>
       <c r="I22" s="1">
         <f>VLOOKUP(A22,'Lawrence Lookups'!V:W,2,FALSE)</f>
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="J22" s="1">
         <f>VLOOKUP(A22,'Lawrence Lookups'!Y:Z,2,FALSE)</f>
@@ -3420,11 +3423,11 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B23" s="1">
         <f>VLOOKUP(A23,'Lawrence Lookups'!A:B,2,FALSE)</f>
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="C23" s="1">
         <f>VLOOKUP(A23,'Lawrence Lookups'!D:E,2,FALSE)</f>
@@ -3432,11 +3435,11 @@
       </c>
       <c r="D23" s="1">
         <f>VLOOKUP(A23,'Lawrence Lookups'!G:H,2,FALSE)</f>
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="E23" s="1">
         <f>VLOOKUP(A23,'Lawrence Lookups'!J:K,2,FALSE)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F23" s="1">
         <f>VLOOKUP(A23,'Lawrence Lookups'!M:N,2,FALSE)</f>
@@ -3444,28 +3447,28 @@
       </c>
       <c r="G23" s="1">
         <f>VLOOKUP('Lawernce Mean Vectors'!A23,'Lawrence Lookups'!P:Q,2,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23" s="1">
         <f>VLOOKUP(A23,'Lawrence Lookups'!S:T,2,FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I23" s="1">
         <f>VLOOKUP(A23,'Lawrence Lookups'!V:W,2,FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J23" s="1">
         <f>VLOOKUP(A23,'Lawrence Lookups'!Y:Z,2,FALSE)</f>
-        <v>-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>40</v>
+      <c r="A24" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="B24" s="1">
         <f>VLOOKUP(A24,'Lawrence Lookups'!A:B,2,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C24" s="1">
         <f>VLOOKUP(A24,'Lawrence Lookups'!D:E,2,FALSE)</f>
@@ -3473,11 +3476,11 @@
       </c>
       <c r="D24" s="1">
         <f>VLOOKUP(A24,'Lawrence Lookups'!G:H,2,FALSE)</f>
-        <v>1.5</v>
+        <v>-1</v>
       </c>
       <c r="E24" s="1">
         <f>VLOOKUP(A24,'Lawrence Lookups'!J:K,2,FALSE)</f>
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="F24" s="1">
         <f>VLOOKUP(A24,'Lawrence Lookups'!M:N,2,FALSE)</f>
@@ -3485,11 +3488,11 @@
       </c>
       <c r="G24" s="1">
         <f>VLOOKUP('Lawernce Mean Vectors'!A24,'Lawrence Lookups'!P:Q,2,FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H24" s="1">
         <f>VLOOKUP(A24,'Lawrence Lookups'!S:T,2,FALSE)</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I24" s="1">
         <f>VLOOKUP(A24,'Lawrence Lookups'!V:W,2,FALSE)</f>
@@ -3500,50 +3503,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B25" s="1">
-        <f>VLOOKUP(A25,'Lawrence Lookups'!A:B,2,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="C25" s="1">
-        <f>VLOOKUP(A25,'Lawrence Lookups'!D:E,2,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="D25" s="1">
-        <f>VLOOKUP(A25,'Lawrence Lookups'!G:H,2,FALSE)</f>
-        <v>-1</v>
-      </c>
-      <c r="E25" s="1">
-        <f>VLOOKUP(A25,'Lawrence Lookups'!J:K,2,FALSE)</f>
-        <v>2</v>
-      </c>
-      <c r="F25" s="1">
-        <f>VLOOKUP(A25,'Lawrence Lookups'!M:N,2,FALSE)</f>
-        <v>2</v>
-      </c>
-      <c r="G25" s="1">
-        <f>VLOOKUP('Lawernce Mean Vectors'!A25,'Lawrence Lookups'!P:Q,2,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="H25" s="1">
-        <f>VLOOKUP(A25,'Lawrence Lookups'!S:T,2,FALSE)</f>
-        <v>-1</v>
-      </c>
-      <c r="I25" s="1">
-        <f>VLOOKUP(A25,'Lawrence Lookups'!V:W,2,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="J25" s="1">
-        <f>VLOOKUP(A25,'Lawrence Lookups'!Y:Z,2,FALSE)</f>
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:J24">
-    <cfRule type="colorScale" priority="10">
+  <conditionalFormatting sqref="B24:J24">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3554,8 +3516,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B25:J25">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="B2:J23">
+    <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3574,8 +3536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Z43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J43" sqref="J43"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="AC13" sqref="AC13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3586,7 +3548,11 @@
     <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.5" customWidth="1"/>
     <col min="16" max="16" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.5" customWidth="1"/>
+    <col min="22" max="22" width="15.5" customWidth="1"/>
+    <col min="25" max="25" width="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.2">
@@ -3877,7 +3843,7 @@
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -3942,13 +3908,13 @@
         <v>39</v>
       </c>
       <c r="H7">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>40</v>
       </c>
       <c r="K7">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>42</v>
@@ -3998,13 +3964,13 @@
         <v>40</v>
       </c>
       <c r="H8">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="J8" t="s">
         <v>8</v>
       </c>
       <c r="K8">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="M8" t="s">
         <v>38</v>
@@ -4044,12 +4010,6 @@
       <c r="B9">
         <v>1</v>
       </c>
-      <c r="D9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9">
-        <v>2</v>
-      </c>
       <c r="G9" t="s">
         <v>14</v>
       </c>
@@ -4113,7 +4073,7 @@
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="K10">
         <v>1</v>
@@ -4122,7 +4082,7 @@
         <v>24</v>
       </c>
       <c r="N10">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="P10" t="s">
         <v>5</v>
@@ -4151,7 +4111,7 @@
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -4178,7 +4138,7 @@
         <v>41</v>
       </c>
       <c r="N11">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="P11" t="s">
         <v>43</v>
@@ -4193,15 +4153,9 @@
         <v>1</v>
       </c>
       <c r="V11" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="W11">
-        <v>1</v>
-      </c>
-      <c r="Y11" t="s">
-        <v>16</v>
-      </c>
-      <c r="Z11">
         <v>1</v>
       </c>
     </row>
@@ -4311,19 +4265,13 @@
         <v>1</v>
       </c>
       <c r="Y13" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="Z13">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
       <c r="D14" t="s">
         <v>20</v>
       </c>
@@ -4336,12 +4284,6 @@
       <c r="H14">
         <v>1</v>
       </c>
-      <c r="J14" t="s">
-        <v>16</v>
-      </c>
-      <c r="K14">
-        <v>1</v>
-      </c>
       <c r="M14" t="s">
         <v>12</v>
       </c>
@@ -4359,12 +4301,6 @@
       </c>
       <c r="T14">
         <v>0</v>
-      </c>
-      <c r="V14" t="s">
-        <v>16</v>
-      </c>
-      <c r="W14">
-        <v>1</v>
       </c>
       <c r="Y14" t="s">
         <v>11</v>
@@ -4399,7 +4335,7 @@
         <v>1</v>
       </c>
       <c r="M15" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="N15">
         <v>0</v>
@@ -4510,12 +4446,6 @@
       <c r="K17">
         <v>0</v>
       </c>
-      <c r="M17" t="s">
-        <v>16</v>
-      </c>
-      <c r="N17">
-        <v>0</v>
-      </c>
       <c r="P17" t="s">
         <v>15</v>
       </c>
@@ -4629,7 +4559,7 @@
         <v>0</v>
       </c>
       <c r="P19" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="Q19">
         <v>-1</v>
@@ -4666,12 +4596,6 @@
       <c r="E20">
         <v>1</v>
       </c>
-      <c r="G20" t="s">
-        <v>16</v>
-      </c>
-      <c r="H20">
-        <v>-1</v>
-      </c>
       <c r="J20" t="s">
         <v>39</v>
       </c>
@@ -4688,12 +4612,6 @@
         <v>11</v>
       </c>
       <c r="Q20">
-        <v>-1</v>
-      </c>
-      <c r="S20" t="s">
-        <v>16</v>
-      </c>
-      <c r="T20">
         <v>-1</v>
       </c>
       <c r="V20" t="s">
@@ -4803,7 +4721,7 @@
         <v>-1</v>
       </c>
       <c r="S22" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="T22">
         <v>-1</v>
@@ -4835,7 +4753,7 @@
         <v>-1</v>
       </c>
       <c r="G23" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="H23">
         <v>-1</v>
@@ -4850,12 +4768,6 @@
         <v>5</v>
       </c>
       <c r="N23">
-        <v>-1</v>
-      </c>
-      <c r="P23" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q23">
         <v>-1</v>
       </c>
       <c r="S23" t="s">

</xml_diff>